<commit_message>
Se hace configuraicon de reporte
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpedraze\IdeaProjects\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4016E34-BB1B-4417-9840-64767D22D52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BB18BF-EDA0-4CEE-BB58-A68728CFDA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -203,6 +203,33 @@
   </si>
   <si>
     <t>29/11/2022</t>
+  </si>
+  <si>
+    <t>16/11/22</t>
+  </si>
+  <si>
+    <t>00:01:22</t>
+  </si>
+  <si>
+    <t>Succes</t>
+  </si>
+  <si>
+    <t>C:\Users\jpedraze\IdeaProjects\everis-app-web-selenium-java-master//reportes//indicadores//16.11.22_20.17.36</t>
+  </si>
+  <si>
+    <t>00:01:59</t>
+  </si>
+  <si>
+    <t>C:\Users\jpedraze\IdeaProjects\everis-app-web-selenium-java-master\reportes\indicadores\16.11.22_20.22.17</t>
+  </si>
+  <si>
+    <t>00:01:20</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>C:\Users\jpedraze\IdeaProjects\everis-app-web-selenium-java-master\reportes\indicadores\16.11.22_21.03.44</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E748D9-ED46-4D76-AD5F-92A006D16DD6}">
   <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1205,7 +1232,7 @@
       </c>
       <c r="F6" s="7">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"succes")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G6" s="7">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"fallo")</f>
@@ -1339,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D82E4AC-5BDA-4423-B100-F014CDDF9FA5}">
   <dimension ref="A1:E401"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1526,15 +1553,55 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="24"/>
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="24"/>

</xml_diff>

<commit_message>
modificacion de esquema escenario cuentas
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>C:\Users\jpedraze\IdeaProjects\everis-app-web-selenium-java-master\reportes\indicadores\16.11.22_21.03.44</t>
+  </si>
+  <si>
+    <t>00:01:11</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\16.11.22_21.35.08</t>
   </si>
 </sst>
 </file>
@@ -1604,8 +1610,21 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="24"/>

</xml_diff>

<commit_message>
Se estabilizan los flujos de cuentas
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -236,6 +236,174 @@
   </si>
   <si>
     <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\16.11.22_21.35.08</t>
+  </si>
+  <si>
+    <t>17/11/22</t>
+  </si>
+  <si>
+    <t>00:02:24</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_09.10.01</t>
+  </si>
+  <si>
+    <t>00:01:24</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_09.14.08</t>
+  </si>
+  <si>
+    <t>00:01:28</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_09.20.52</t>
+  </si>
+  <si>
+    <t>00:02:18</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_09.27.12</t>
+  </si>
+  <si>
+    <t>00:00:48</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_09.47.39</t>
+  </si>
+  <si>
+    <t>00:00:52</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_11.45.13</t>
+  </si>
+  <si>
+    <t>00:00:25</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.09.15</t>
+  </si>
+  <si>
+    <t>00:00:45</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.11.02</t>
+  </si>
+  <si>
+    <t>00:00:41</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.13.55</t>
+  </si>
+  <si>
+    <t>00:00:47</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.18.31</t>
+  </si>
+  <si>
+    <t>00:01:25</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.28.45</t>
+  </si>
+  <si>
+    <t>00:01:19</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.45.10</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.47.28</t>
+  </si>
+  <si>
+    <t>00:00:18</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.50.33</t>
+  </si>
+  <si>
+    <t>00:01:26</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.52.42</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_14.59.50</t>
+  </si>
+  <si>
+    <t>00:01:29</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_15.02.08</t>
+  </si>
+  <si>
+    <t>00:01:31</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_15.08.01</t>
+  </si>
+  <si>
+    <t>00:02:16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_15.10.19</t>
+  </si>
+  <si>
+    <t>00:00:44</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_15.23.28</t>
+  </si>
+  <si>
+    <t>00:01:13</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_16.36.44</t>
+  </si>
+  <si>
+    <t>00:01:17</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_16.38.58</t>
+  </si>
+  <si>
+    <t>00:01:21</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_16.47.36</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_16.49.56</t>
+  </si>
+  <si>
+    <t>00:00:40</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_17.07.27</t>
+  </si>
+  <si>
+    <t>00:00:50</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_17.09.05</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_17.18.16</t>
+  </si>
+  <si>
+    <t>00:00:58</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\17.11.22_19.10.45</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1449,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99C41C1-9AE8-4879-9151-AF8CDA72B09F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -1295,16 +1463,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>33</v>
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1627,32 +1798,123 @@
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="24"/>
@@ -3167,7 +3429,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4BB373-E012-4B33-A2CA-3C06D5457D5C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3181,16 +3443,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>33</v>
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cambios 24/11/2022 / 11 am
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alkosto\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A673B-6680-4CF1-A607-4540F7D57AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D24A74-0AE7-4949-9E44-732817450878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="1" activeTab="4" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="6" activeTab="10" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,18 @@
     <sheet name="CreacionCuentaAliados" sheetId="4" r:id="rId4"/>
     <sheet name="CreacionCuentaEmpresa" sheetId="6" r:id="rId5"/>
     <sheet name="CreacionCuentaPersonas" sheetId="7" r:id="rId6"/>
+    <sheet name="CreacionCasoFelicitaciones" sheetId="8" r:id="rId7"/>
+    <sheet name="creacionCasoInformacion" sheetId="9" r:id="rId8"/>
+    <sheet name="creacionCasoQueja" sheetId="10" r:id="rId9"/>
+    <sheet name="creacionCasoSolicitud" sheetId="11" r:id="rId10"/>
+    <sheet name="creacionCasoSugerencia" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CreacionCuentaEmpresa!$A$1:$E$16</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -194,6 +199,18 @@
   </si>
   <si>
     <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.26.55</t>
+  </si>
+  <si>
+    <t>CreacionCasoFelicitaciones</t>
+  </si>
+  <si>
+    <t>CreacionCasoInformacion</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\24.11.22_08.50.24</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\24.11.22_08.52.15</t>
   </si>
 </sst>
 </file>
@@ -459,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -504,14 +521,22 @@
     <xf numFmtId="21" fontId="7" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,16 +557,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,21 +879,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F4" s="13" t="s">
@@ -958,6 +973,440 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF4948-357F-40F6-A41C-D62917141212}">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="54"/>
+      <c r="C32" s="55"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="54"/>
+      <c r="C33" s="55"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="54"/>
+      <c r="C34" s="55"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="54"/>
+      <c r="C35" s="55"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63BF217-BF6E-441B-AE01-3F0540C3AB75}">
+  <dimension ref="A1:E56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="5" max="5" width="80.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="54"/>
+      <c r="C32" s="55"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="54"/>
+      <c r="C33" s="55"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="54"/>
+      <c r="C34" s="55"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="54"/>
+      <c r="C35" s="55"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="54"/>
+      <c r="C37" s="55"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="54"/>
+      <c r="C38" s="55"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="54"/>
+      <c r="C39" s="55"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="54"/>
+      <c r="C40" s="55"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="54"/>
+      <c r="C41" s="55"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="54"/>
+      <c r="C42" s="55"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="54"/>
+      <c r="C43" s="55"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="54"/>
+      <c r="C44" s="55"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="54"/>
+      <c r="C45" s="55"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="54"/>
+      <c r="C46" s="55"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="54"/>
+      <c r="C47" s="55"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="54"/>
+      <c r="C48" s="55"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="54"/>
+      <c r="C49" s="55"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="54"/>
+      <c r="C50" s="55"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="54"/>
+      <c r="C51" s="55"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="54"/>
+      <c r="C52" s="55"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="54"/>
+      <c r="C53" s="55"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="54"/>
+      <c r="C54" s="55"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="54"/>
+      <c r="C55" s="55"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="54"/>
+      <c r="C56" s="55"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -971,10 +1420,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="47.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="46.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
@@ -1002,7 +1451,7 @@
       </c>
     </row>
     <row r="3" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1020,7 +1469,7 @@
       </c>
     </row>
     <row r="4" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1485,7 @@
       </c>
     </row>
     <row r="5" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1049,7 +1498,7 @@
       </c>
     </row>
     <row r="6" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1511,7 @@
       </c>
     </row>
     <row r="7" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1525,7 @@
       </c>
     </row>
     <row r="8" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="59" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1091,7 +1540,7 @@
       </c>
     </row>
     <row r="9" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1553,7 @@
       </c>
     </row>
     <row r="10" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1160,26 +1609,26 @@
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -1232,15 +1681,15 @@
       </c>
       <c r="C6" s="34">
         <f>COUNTIF(CreacionCuentaEmpresa!A2:A13,"CreacionCuentaEmpresa")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="36">
         <f>MAX(CreacionCuentaEmpresa!C2:C8)</f>
-        <v>0</v>
+        <v>44887.000771423613</v>
       </c>
       <c r="E6" s="36">
         <f>MIN(CreacionCuentaEmpresa!C2:C22)</f>
-        <v>0</v>
+        <v>44887.000656550925</v>
       </c>
       <c r="F6" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"SUCCES")</f>
@@ -1248,7 +1697,7 @@
       </c>
       <c r="G6" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"FAILED")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1273,6 +1722,56 @@
       </c>
       <c r="G7" s="37">
         <f>COUNTIF(CreacionCuentaPersonas!D3:D17,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="34">
+        <f>COUNTIF(CreacionCasoFelicitaciones!A4:A24,"creacionCasoFelicitaciones")</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="36">
+        <f>MAX(CreacionCasoFelicitaciones!C3:C62)</f>
+        <v>44889.000517777778</v>
+      </c>
+      <c r="E8" s="36">
+        <f>MIN(CreacionCasoFelicitaciones!C3:C32)</f>
+        <v>44889.000517777778</v>
+      </c>
+      <c r="F8" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D4:D21,"SUCCES")</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D4:D18,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="34">
+        <f>COUNTIF(creacionCasoInformacion!A5:A25,"creacionCasoInformacions")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="36">
+        <f>MAX(CreacionCasoFelicitaciones!C4:C63)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="36">
+        <f>MIN(CreacionCasoFelicitaciones!C4:C33)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D5:D22,"SUCCES")</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D5:D19,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
@@ -1299,10 +1798,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="97.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="97.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,15 +2056,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D82E4AC-5BDA-4423-B100-F014CDDF9FA5}">
   <dimension ref="A1:E401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="95.140625" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="95.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,11 +2088,11 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="54" t="n">
+      <c r="B2" s="42">
         <v>44887.628338333336</v>
       </c>
-      <c r="C2" s="55" t="n">
-        <v>44887.00066142361</v>
+      <c r="C2" s="43">
+        <v>44887.000661423612</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
@@ -1606,11 +2105,11 @@
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="56" t="n">
-        <v>44887.62942346065</v>
-      </c>
-      <c r="C3" s="57" t="n">
-        <v>44887.00072458333</v>
+      <c r="B3" s="44">
+        <v>44887.629423460647</v>
+      </c>
+      <c r="C3" s="45">
+        <v>44887.000724583333</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -1623,11 +2122,11 @@
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="58" t="n">
-        <v>44887.63049549769</v>
-      </c>
-      <c r="C4" s="59" t="n">
-        <v>44887.00077142361</v>
+      <c r="B4" s="46">
+        <v>44887.630495497688</v>
+      </c>
+      <c r="C4" s="47">
+        <v>44887.000771423613</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -1640,10 +2139,10 @@
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="60" t="n">
+      <c r="B5" s="48">
         <v>44887.643097789354</v>
       </c>
-      <c r="C5" s="61" t="n">
+      <c r="C5" s="49">
         <v>44887.000656550925</v>
       </c>
       <c r="D5" t="s">
@@ -1657,11 +2156,11 @@
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="62" t="n">
-        <v>44887.64448542824</v>
-      </c>
-      <c r="C6" s="63" t="n">
-        <v>44887.00076883102</v>
+      <c r="B6" s="50">
+        <v>44887.644485428238</v>
+      </c>
+      <c r="C6" s="51">
+        <v>44887.000768831022</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -1671,16 +2170,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="39"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="42"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
@@ -3263,14 +3762,14 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="97.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="97.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,4 +4088,473 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD12C50-8006-4482-89FC-B707702EBA26}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="91.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="52">
+        <v>44889.36891646991</v>
+      </c>
+      <c r="C2" s="53">
+        <v>44889.000548587966</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="54">
+        <v>44889.370155092591</v>
+      </c>
+      <c r="C3" s="55">
+        <v>44889.000517777778</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B796CB-0EB1-42DF-9E74-36B105845987}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="80.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0E75C9-AD9E-493F-9E18-B1F69B9E3651}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios 29/11/22 - 11:30
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alkosto\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D24A74-0AE7-4949-9E44-732817450878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612C7C54-66BF-484E-8DA6-46E38ADC1228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="6" activeTab="10" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="CreacionCuentaEmpresa" sheetId="6" r:id="rId5"/>
     <sheet name="CreacionCuentaPersonas" sheetId="7" r:id="rId6"/>
     <sheet name="CreacionCasoFelicitaciones" sheetId="8" r:id="rId7"/>
-    <sheet name="creacionCasoInformacion" sheetId="9" r:id="rId8"/>
+    <sheet name="CreacionCasoInformacion" sheetId="9" r:id="rId8"/>
     <sheet name="creacionCasoQueja" sheetId="10" r:id="rId9"/>
     <sheet name="creacionCasoSolicitud" sheetId="11" r:id="rId10"/>
     <sheet name="creacionCasoSugerencia" sheetId="12" r:id="rId11"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -183,34 +183,46 @@
     <t>ruta</t>
   </si>
   <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.03.49</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.05.17</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.06.46</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.25.05</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\22.11.22_15.26.55</t>
-  </si>
-  <si>
     <t>CreacionCasoFelicitaciones</t>
   </si>
   <si>
     <t>CreacionCasoInformacion</t>
   </si>
   <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\24.11.22_08.50.24</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\24.11.22_08.52.15</t>
+    <t>Se crea caso felicitaciones</t>
+  </si>
+  <si>
+    <t>CreacionCasoQueja</t>
+  </si>
+  <si>
+    <t>CreacionCasoSolicitud</t>
+  </si>
+  <si>
+    <t>CreacionCasoSugerencia</t>
+  </si>
+  <si>
+    <t>creacionCasoSugerencia</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\29.11.22_11.15.16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\29.11.22_11.18.37</t>
+  </si>
+  <si>
+    <t>Se crea caso informacion</t>
+  </si>
+  <si>
+    <t>Se crea caso solicitud</t>
+  </si>
+  <si>
+    <t>Se crea caso queja</t>
+  </si>
+  <si>
+    <t>Se crea caso sugerencia</t>
   </si>
 </sst>
 </file>
@@ -476,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -521,16 +533,6 @@
     <xf numFmtId="21" fontId="7" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -557,6 +559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +877,7 @@
   <dimension ref="F3:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,13 +890,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F4" s="13" t="s">
@@ -917,15 +920,15 @@
         <v>24</v>
       </c>
       <c r="G5" s="19">
-        <f>ServiceCloud!C11</f>
-        <v>6</v>
+        <f>ServiceCloud!C16</f>
+        <v>11</v>
       </c>
       <c r="H5" s="12">
-        <f>1-(ServiceCloud!D11)</f>
+        <f>1-(ServiceCloud!D16)</f>
         <v>0</v>
       </c>
       <c r="I5" s="12">
-        <f>ServiceCloud!D11</f>
+        <f>ServiceCloud!D16</f>
         <v>1</v>
       </c>
       <c r="J5" s="15" t="s">
@@ -955,7 +958,7 @@
       </c>
       <c r="G7" s="16">
         <f>SUM(G5:G6)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H7" s="17">
         <f>SUM(H5:H6)</f>
@@ -981,7 +984,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E36"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,148 +1011,197 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
-      <c r="C23" s="55"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="54"/>
-      <c r="C32" s="55"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1157,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63BF217-BF6E-441B-AE01-3F0540C3AB75}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,243 +1237,312 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
+      <c r="A2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="42">
+        <v>44894.469818263889</v>
+      </c>
+      <c r="C2" s="43">
+        <v>44894.000859594904</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
+      <c r="A3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="44">
+        <v>44894.472174861112</v>
+      </c>
+      <c r="C3" s="45">
+        <v>44894.000888449074</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
-      <c r="C23" s="55"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="54"/>
-      <c r="C32" s="55"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="54"/>
-      <c r="C37" s="55"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="41"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="54"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="54"/>
-      <c r="C39" s="55"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="54"/>
-      <c r="C40" s="55"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="41"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="54"/>
-      <c r="C42" s="55"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="41"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="54"/>
-      <c r="C43" s="55"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="41"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="54"/>
-      <c r="C44" s="55"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="41"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="54"/>
-      <c r="C45" s="55"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="54"/>
-      <c r="C46" s="55"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="41"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="54"/>
-      <c r="C47" s="55"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="54"/>
-      <c r="C48" s="55"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="54"/>
-      <c r="C49" s="55"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="41"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="54"/>
-      <c r="C50" s="55"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="54"/>
-      <c r="C51" s="55"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="54"/>
-      <c r="C52" s="55"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="54"/>
-      <c r="C53" s="55"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="54"/>
-      <c r="C54" s="55"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="54"/>
-      <c r="C55" s="55"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="41"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="54"/>
-      <c r="C56" s="55"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B430242B-CBFC-46E1-B24F-A7821E356ECB}">
-  <dimension ref="A1:XFC14"/>
+  <dimension ref="A1:XFC18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="46.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -1451,7 +1572,7 @@
       </c>
     </row>
     <row r="3" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1469,7 +1590,7 @@
       </c>
     </row>
     <row r="4" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1477,7 +1598,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="12">
-        <f t="shared" ref="D4:D6" si="0">IF(C4="Si",100%,0%)</f>
+        <f t="shared" ref="D4:D11" si="0">IF(C4="Si",100%,0%)</f>
         <v>1</v>
       </c>
       <c r="XFC4" t="s">
@@ -1485,7 +1606,7 @@
       </c>
     </row>
     <row r="5" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1498,7 +1619,7 @@
       </c>
     </row>
     <row r="6" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1511,91 +1632,153 @@
       </c>
     </row>
     <row r="7" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
-      <c r="B7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="8">
-        <f>COUNTIF(C3:C6,"Si")+COUNTIF(C3:C6,"No")</f>
-        <v>4</v>
-      </c>
-      <c r="D7" s="20">
-        <f>SUM(D3:D6)/C7</f>
+      <c r="A7" s="50"/>
+      <c r="B7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
+      <c r="A8" s="50"/>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="12">
-        <f>IF(C8="Si",100%,0%)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="7" t="s">
-        <v>3</v>
+      <c r="A9" s="50"/>
+      <c r="B9" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="12">
-        <f>IF(C9="Si",100%,0%)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8">
+        <f>COUNTIF(C3:C11,"Si")+COUNTIF(C3:C11,"No")</f>
+        <v>9</v>
+      </c>
+      <c r="D12" s="20">
+        <f>SUM(D3:D11)/C12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="12">
+        <f>IF(C13="Si",100%,0%)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="12">
+        <f>IF(C14="Si",100%,0%)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
-        <f>COUNTIF(C8:C9,"Si")+COUNTIF(C8:C9,"No")</f>
+      <c r="C15" s="8">
+        <f>COUNTIF(C13:C14,"Si")+COUNTIF(C13:C14,"No")</f>
         <v>2</v>
       </c>
-      <c r="D10" s="20">
-        <f>SUM(D8:D9)/C10</f>
+      <c r="D15" s="20">
+        <f>SUM(D13:D14)/C15</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="9" t="s">
+    <row r="16" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9">
-        <f>SUM(C10,C7)</f>
-        <v>6</v>
-      </c>
-      <c r="D11" s="11">
-        <f>SUM(D7,D10)/2</f>
+      <c r="C16" s="9">
+        <f>SUM(C15,C12)</f>
+        <v>11</v>
+      </c>
+      <c r="D16" s="11">
+        <f>SUM(D12,D15)/2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-    </row>
-    <row r="14" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8:C9" xr:uid="{8C893A13-FD0D-4583-A29B-99FBAB08404C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14 C3:C11" xr:uid="{8C893A13-FD0D-4583-A29B-99FBAB08404C}">
       <formula1>$XFC$3:$XFC$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -1609,7 +1792,7 @@
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,13 +1805,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -1681,15 +1864,15 @@
       </c>
       <c r="C6" s="34">
         <f>COUNTIF(CreacionCuentaEmpresa!A2:A13,"CreacionCuentaEmpresa")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="36">
         <f>MAX(CreacionCuentaEmpresa!C2:C8)</f>
-        <v>44887.000771423613</v>
+        <v>0</v>
       </c>
       <c r="E6" s="36">
         <f>MIN(CreacionCuentaEmpresa!C2:C22)</f>
-        <v>44887.000656550925</v>
+        <v>0</v>
       </c>
       <c r="F6" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"SUCCES")</f>
@@ -1697,7 +1880,7 @@
       </c>
       <c r="G6" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"FAILED")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1726,8 +1909,8 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>50</v>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(CreacionCasoFelicitaciones!A4:A24,"creacionCasoFelicitaciones")</f>
@@ -1735,11 +1918,11 @@
       </c>
       <c r="D8" s="36">
         <f>MAX(CreacionCasoFelicitaciones!C3:C62)</f>
-        <v>44889.000517777778</v>
+        <v>0</v>
       </c>
       <c r="E8" s="36">
         <f>MIN(CreacionCasoFelicitaciones!C3:C32)</f>
-        <v>44889.000517777778</v>
+        <v>0</v>
       </c>
       <c r="F8" s="37">
         <f>COUNTIF(CreacionCasoFelicitaciones!D4:D21,"SUCCES")</f>
@@ -1751,27 +1934,102 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>51</v>
+      <c r="B9" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="34">
-        <f>COUNTIF(creacionCasoInformacion!A5:A25,"creacionCasoInformacions")</f>
+        <f>COUNTIF(CreacionCasoInformacion!A5:A25,"creacionCasoInformacion")</f>
         <v>0</v>
       </c>
       <c r="D9" s="36">
-        <f>MAX(CreacionCasoFelicitaciones!C4:C63)</f>
+        <f>MAX(CreacionCasoInformacion!C4:C63)</f>
         <v>0</v>
       </c>
       <c r="E9" s="36">
-        <f>MIN(CreacionCasoFelicitaciones!C4:C33)</f>
+        <f>MIN(CreacionCasoInformacion!C4:C33)</f>
         <v>0</v>
       </c>
       <c r="F9" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D5:D22,"SUCCES")</f>
+        <f>COUNTIF(CreacionCasoInformacion!D5:D22,"SUCCES")</f>
         <v>0</v>
       </c>
       <c r="G9" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D5:D19,"FAILED")</f>
+        <f>COUNTIF(CreacionCasoInformacion!D5:D19,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="34">
+        <f>COUNTIF(creacionCasoQueja!A6:A26,"creacionCasoQueja")</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="36">
+        <f>MAX(creacionCasoQueja!C5:C64)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="36">
+        <f>MIN(creacionCasoQueja!C5:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="37">
+        <f>COUNTIF(creacionCasoQueja!D6:D23,"SUCCES")</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="37">
+        <f>COUNTIF(creacionCasoQueja!D6:D20,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="34">
+        <f>COUNTIF(creacionCasoSolicitud!A7:A27,"creacionCasoSolicitud")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="36">
+        <f>MAX(creacionCasoSolicitud!C6:C65)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="36">
+        <f>MIN(CreacionCasoFelicitaciones!C6:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="37">
+        <f>COUNTIF(creacionCasoSolicitud!D7:D24,"SUCCES")</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="37">
+        <f>COUNTIF(creacionCasoSolicitud!D7:D21,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="34">
+        <f>COUNTIF(creacionCasoSugerencia!A8:A28,"creacionCasoSugerencia")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="36">
+        <f>MAX(creacionCasoSugerencia!C7:C66)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="36">
+        <f>MIN(creacionCasoSugerencia!C7:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="37">
+        <f>COUNTIF(creacionCasoSugerencia!D8:D25,"SUCCES")</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="37">
+        <f>COUNTIF(creacionCasoSugerencia!D8:D22,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
@@ -2057,7 +2315,7 @@
   <dimension ref="A1:E401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E6"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,191 +2343,174 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="42">
-        <v>44887.628338333336</v>
-      </c>
-      <c r="C2" s="43">
-        <v>44887.000661423612</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="44">
-        <v>44887.629423460647</v>
-      </c>
-      <c r="C3" s="45">
-        <v>44887.000724583333</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="46">
-        <v>44887.630495497688</v>
-      </c>
-      <c r="C4" s="47">
-        <v>44887.000771423613</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="48">
-        <v>44887.643097789354</v>
-      </c>
-      <c r="C5" s="49">
-        <v>44887.000656550925</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="50">
-        <v>44887.644485428238</v>
-      </c>
-      <c r="C6" s="51">
-        <v>44887.000768831022</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
-      <c r="C8" s="39"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="24"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="24"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="24"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="24"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="24"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="24"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="24"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="24"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
       <c r="C24" s="24"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="24"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="24"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="24"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="24"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="24"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
       <c r="C31" s="24"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="24"/>
     </row>
@@ -3762,7 +4003,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4095,7 +4336,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4124,146 +4365,168 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="52">
-        <v>44889.36891646991</v>
-      </c>
-      <c r="C2" s="53">
-        <v>44889.000548587966</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="54">
-        <v>44889.370155092591</v>
-      </c>
-      <c r="C3" s="55">
-        <v>44889.000517777778</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4274,10 +4537,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B796CB-0EB1-42DF-9E74-36B105845987}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E23"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4305,92 +4568,188 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
-      <c r="C23" s="55"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4404,7 +4763,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E31"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4434,127 +4793,176 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
-      <c r="C20" s="55"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
-      <c r="C23" s="55"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios 30/11/22 - 03:53 PM
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -8,25 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alkosto\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612C7C54-66BF-484E-8DA6-46E38ADC1228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91AB22-655C-41E2-84AE-06DBE16AA577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="2" activeTab="2" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
     <sheet name="ServiceCloud" sheetId="2" r:id="rId2"/>
     <sheet name="Indicadores de ejecucion" sheetId="5" r:id="rId3"/>
-    <sheet name="CreacionCuentaAliados" sheetId="4" r:id="rId4"/>
-    <sheet name="CreacionCuentaEmpresa" sheetId="6" r:id="rId5"/>
-    <sheet name="CreacionCuentaPersonas" sheetId="7" r:id="rId6"/>
-    <sheet name="CreacionCasoFelicitaciones" sheetId="8" r:id="rId7"/>
-    <sheet name="CreacionCasoInformacion" sheetId="9" r:id="rId8"/>
-    <sheet name="creacionCasoQueja" sheetId="10" r:id="rId9"/>
-    <sheet name="creacionCasoSolicitud" sheetId="11" r:id="rId10"/>
-    <sheet name="creacionCasoSugerencia" sheetId="12" r:id="rId11"/>
+    <sheet name="inicioSesionExitoso" sheetId="15" r:id="rId4"/>
+    <sheet name="inicioSesionFallido" sheetId="14" r:id="rId5"/>
+    <sheet name="CreacionCuentaAliados" sheetId="4" r:id="rId6"/>
+    <sheet name="CreacionCuentaEmpresa" sheetId="6" r:id="rId7"/>
+    <sheet name="CreacionCuentaPersonas" sheetId="7" r:id="rId8"/>
+    <sheet name="cuentaExistente" sheetId="13" r:id="rId9"/>
+    <sheet name="creaCuentaDesdeCasos" sheetId="16" r:id="rId10"/>
+    <sheet name="CreacionCasoFelicitaciones" sheetId="8" r:id="rId11"/>
+    <sheet name="CreacionCasoInformacion" sheetId="9" r:id="rId12"/>
+    <sheet name="creacionCasoQueja" sheetId="10" r:id="rId13"/>
+    <sheet name="creacionCasoSolicitud" sheetId="11" r:id="rId14"/>
+    <sheet name="creacionCasoSugerencia" sheetId="12" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CreacionCuentaEmpresa!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CreacionCuentaEmpresa!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -177,9 +181,6 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>CreacionCuentaPersona</t>
-  </si>
-  <si>
     <t>ruta</t>
   </si>
   <si>
@@ -201,28 +202,85 @@
     <t>CreacionCasoSugerencia</t>
   </si>
   <si>
+    <t>Se crea caso informacion</t>
+  </si>
+  <si>
+    <t>Se crea caso solicitud</t>
+  </si>
+  <si>
+    <t>Se crea caso queja</t>
+  </si>
+  <si>
+    <t>Se crea caso sugerencia</t>
+  </si>
+  <si>
+    <t>Crea Cuenta desde la creacion de casos</t>
+  </si>
+  <si>
+    <t>inicioSesionExitoso</t>
+  </si>
+  <si>
+    <t>inicioSesionFallido</t>
+  </si>
+  <si>
+    <t>cuentaExistente</t>
+  </si>
+  <si>
+    <t>creaCuentaDesdeCasos</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.16.11</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.17.03</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.18.38</t>
+  </si>
+  <si>
+    <t>CreacionCuentaPersonas</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.20.03</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.24.54</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.26.47</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.28.04</t>
+  </si>
+  <si>
     <t>creacionCasoSugerencia</t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\29.11.22_11.15.16</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\29.11.22_11.18.37</t>
-  </si>
-  <si>
-    <t>Se crea caso informacion</t>
-  </si>
-  <si>
-    <t>Se crea caso solicitud</t>
-  </si>
-  <si>
-    <t>Se crea caso queja</t>
-  </si>
-  <si>
-    <t>Se crea caso sugerencia</t>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.29.50</t>
+  </si>
+  <si>
+    <t>creacionCasoSolicitud</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.31.39</t>
+  </si>
+  <si>
+    <t>creacionCasoQueja</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.33.50</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.35.37</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.38.30</t>
   </si>
 </sst>
 </file>
@@ -488,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -539,6 +597,35 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -559,7 +646,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +963,7 @@
   <dimension ref="F3:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,13 +976,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F4" s="13" t="s">
@@ -920,15 +1006,15 @@
         <v>24</v>
       </c>
       <c r="G5" s="19">
-        <f>ServiceCloud!C16</f>
-        <v>11</v>
+        <f>ServiceCloud!C17</f>
+        <v>12</v>
       </c>
       <c r="H5" s="12">
-        <f>1-(ServiceCloud!D16)</f>
+        <f>1-(ServiceCloud!D17)</f>
         <v>0</v>
       </c>
       <c r="I5" s="12">
-        <f>ServiceCloud!D16</f>
+        <f>ServiceCloud!D17</f>
         <v>1</v>
       </c>
       <c r="J5" s="15" t="s">
@@ -958,7 +1044,7 @@
       </c>
       <c r="G7" s="16">
         <f>SUM(G5:G6)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="17">
         <f>SUM(H5:H6)</f>
@@ -980,6 +1066,810 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB547C11-8059-4516-AEFD-2AA57D4205D1}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="84.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="63">
+        <v>44895.645306481485</v>
+      </c>
+      <c r="C2" s="64">
+        <v>44895.000791342594</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD12C50-8006-4482-89FC-B707702EBA26}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="91.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="73">
+        <v>44895.652058402775</v>
+      </c>
+      <c r="C2" s="74">
+        <v>44895.000289386575</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B796CB-0EB1-42DF-9E74-36B105845987}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="88.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="71">
+        <v>44895.650510613428</v>
+      </c>
+      <c r="C2" s="72">
+        <v>44895.000761944444</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0E75C9-AD9E-493F-9E18-B1F69B9E3651}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="82.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="69">
+        <v>44895.649289513887</v>
+      </c>
+      <c r="C2" s="70">
+        <v>44895.000770451392</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF4948-357F-40F6-A41C-D62917141212}">
   <dimension ref="A1:E36"/>
   <sheetViews>
@@ -989,8 +1879,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="82.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="82.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,15 +1897,25 @@
         <v>33</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="67">
+        <v>44895.64780835648</v>
+      </c>
+      <c r="C2" s="68">
+        <v>44895.00081622685</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
@@ -1205,18 +2105,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63BF217-BF6E-441B-AE01-3F0540C3AB75}">
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="5" max="5" width="80.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="80.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,42 +2133,32 @@
         <v>33</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="42">
-        <v>44894.469818263889</v>
-      </c>
-      <c r="C2" s="43">
-        <v>44894.000859594904</v>
+        <v>68</v>
+      </c>
+      <c r="B2" s="65">
+        <v>44895.646562002315</v>
+      </c>
+      <c r="C2" s="66">
+        <v>44895.000819166664</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="44">
-        <v>44894.472174861112</v>
-      </c>
-      <c r="C3" s="45">
-        <v>44894.000888449074</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>53</v>
-      </c>
+      <c r="A3" s="28"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
@@ -1533,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B430242B-CBFC-46E1-B24F-A7821E356ECB}">
-  <dimension ref="A1:XFC18"/>
+  <dimension ref="A1:XFC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +2462,7 @@
       </c>
     </row>
     <row r="3" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="78" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1590,7 +2480,7 @@
       </c>
     </row>
     <row r="4" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
+      <c r="A4" s="79"/>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +2488,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="12">
-        <f t="shared" ref="D4:D11" si="0">IF(C4="Si",100%,0%)</f>
+        <f t="shared" ref="D4:D12" si="0">IF(C4="Si",100%,0%)</f>
         <v>1</v>
       </c>
       <c r="XFC4" t="s">
@@ -1606,7 +2496,7 @@
       </c>
     </row>
     <row r="5" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="79"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1619,7 +2509,7 @@
       </c>
     </row>
     <row r="6" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1632,22 +2522,21 @@
       </c>
     </row>
     <row r="7" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="12">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>26</v>
@@ -1658,9 +2547,9 @@
       </c>
     </row>
     <row r="9" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>26</v>
@@ -1671,9 +2560,9 @@
       </c>
     </row>
     <row r="10" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="52" t="s">
-        <v>55</v>
+      <c r="A10" s="79"/>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
@@ -1684,9 +2573,9 @@
       </c>
     </row>
     <row r="11" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="6" t="s">
-        <v>57</v>
+      <c r="A11" s="79"/>
+      <c r="B11" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>26</v>
@@ -1697,38 +2586,38 @@
       </c>
     </row>
     <row r="12" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="80"/>
+      <c r="B12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8">
-        <f>COUNTIF(C3:C11,"Si")+COUNTIF(C3:C11,"No")</f>
-        <v>9</v>
-      </c>
-      <c r="D12" s="20">
-        <f>SUM(D3:D11)/C12</f>
+      <c r="C13" s="8">
+        <f>COUNTIF(C3:C12,"Si")+COUNTIF(C3:C12,"No")</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="20">
+        <f>SUM(D3:D12)/C13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="79"/>
+      <c r="B14" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="12">
-        <f>IF(C13="Si",100%,0%)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>26</v>
@@ -1739,46 +2628,59 @@
       </c>
     </row>
     <row r="15" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="8">
-        <f>COUNTIF(C13:C14,"Si")+COUNTIF(C13:C14,"No")</f>
-        <v>2</v>
-      </c>
-      <c r="D15" s="20">
-        <f>SUM(D13:D14)/C15</f>
+      <c r="A15" s="79"/>
+      <c r="B15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="12">
+        <f>IF(C15="Si",100%,0%)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8">
+        <f>COUNTIF(C14:C15,"Si")+COUNTIF(C14:C15,"No")</f>
+        <v>2</v>
+      </c>
+      <c r="D16" s="20">
+        <f>SUM(D14:D15)/C16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9">
-        <f>SUM(C15,C12)</f>
-        <v>11</v>
-      </c>
-      <c r="D16" s="11">
-        <f>SUM(D12,D15)/2</f>
+      <c r="C17" s="9">
+        <f>SUM(C16,C13)</f>
+        <v>12</v>
+      </c>
+      <c r="D17" s="11">
+        <f>SUM(D13,D16)/2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14 C3:C11" xr:uid="{8C893A13-FD0D-4583-A29B-99FBAB08404C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C15 C3:C12" xr:uid="{8C893A13-FD0D-4583-A29B-99FBAB08404C}">
       <formula1>$XFC$3:$XFC$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -1789,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E748D9-ED46-4D76-AD5F-92A006D16DD6}">
-  <dimension ref="B3:G15"/>
+  <dimension ref="B3:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,13 +2707,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -1835,207 +2737,307 @@
     </row>
     <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="34">
+        <f>COUNTIF(inicioSesionExitoso!A1:A16,"inicioSesionExitoso")</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="35">
+        <f>MAX(inicioSesionExitoso!C1:C94)</f>
+        <v>44895.000122928242</v>
+      </c>
+      <c r="E5" s="36">
+        <f>MIN(inicioSesionExitoso!C1:C20)</f>
+        <v>44895.000122928242</v>
+      </c>
+      <c r="F5" s="37">
+        <f>COUNTIF(inicioSesionExitoso!D1:D17,"PASSED")</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="37">
+        <f>COUNTIF(inicioSesionExitoso!D1:D21,"FAILED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="34">
+        <f>COUNTIF(inicioSesionFallido!A2:A17,"inicioSesionFallido")</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="35">
+        <f>MAX(inicioSesionFallido!C2:C95)</f>
+        <v>44895.000157627313</v>
+      </c>
+      <c r="E6" s="36">
+        <f>MIN(inicioSesionFallido!C2:C21)</f>
+        <v>44895.000157627313</v>
+      </c>
+      <c r="F6" s="37">
+        <f>COUNTIF(inicioSesionFallido!D2:D18,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="37">
+        <f>COUNTIF(inicioSesionFallido!D2:D22,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C7" s="34">
         <f>COUNTIF(CreacionCuentaAliados!A2:A17,"CreacionCuentaAliados")</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="35">
+        <v>1</v>
+      </c>
+      <c r="D7" s="35">
         <f>MAX(CreacionCuentaAliados!C2:C95)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="36">
+        <v>44895.000453946763</v>
+      </c>
+      <c r="E7" s="36">
         <f>MIN(CreacionCuentaAliados!C2:C21)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="37">
+        <v>44895.000453946763</v>
+      </c>
+      <c r="F7" s="37">
         <f>COUNTIF(CreacionCuentaAliados!D2:D18,"SUCCES")</f>
         <v>0</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G7" s="37">
         <f>COUNTIF(CreacionCuentaAliados!D2:D22,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="34">
+        <f>COUNTIF(CreacionCuentaEmpresa!A2:A13,"CreacionCuentaEmpresa")</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="36">
+        <f>MAX(CreacionCuentaEmpresa!C2:C8)</f>
+        <v>44895.000818958331</v>
+      </c>
+      <c r="E8" s="36">
+        <f>MIN(CreacionCuentaEmpresa!C2:C22)</f>
+        <v>44895.000818958331</v>
+      </c>
+      <c r="F8" s="37">
+        <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"PASSED")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="34">
-        <f>COUNTIF(CreacionCuentaEmpresa!A2:A13,"CreacionCuentaEmpresa")</f>
+      <c r="G8" s="37">
+        <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="34">
+        <f>COUNTIF(CreacionCuentaPersonas!A2:A14,"CreacionCuentaPersonas")</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="36">
+        <f>MAX(CreacionCuentaPersonas!C2:C8)</f>
+        <v>44895.000503796298</v>
+      </c>
+      <c r="E9" s="36">
+        <f>MIN(CreacionCuentaPersonas!C2:C23)</f>
+        <v>44895.000503796298</v>
+      </c>
+      <c r="F9" s="37">
+        <f>COUNTIF(CreacionCuentaPersonas!D2:D19,"PASSED")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="36">
-        <f>MAX(CreacionCuentaEmpresa!C2:C8)</f>
+      <c r="G9" s="37">
+        <f>COUNTIF(CreacionCuentaPersonas!D2:D13,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="34">
+        <f>COUNTIF(cuentaExistente!A2:A15,"cuentaExistente")</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="36">
+        <f>MAX(cuentaExistente!C2:C10)</f>
+        <v>44895.000481504627</v>
+      </c>
+      <c r="E10" s="36">
+        <f>MIN(cuentaExistente!C2:C24)</f>
+        <v>44895.000481504627</v>
+      </c>
+      <c r="F10" s="37">
+        <f>COUNTIF(cuentaExistente!D2:D20,"PASSED")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="36">
-        <f>MIN(CreacionCuentaEmpresa!C2:C22)</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="37">
-        <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"SUCCES")</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="37">
-        <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="34">
-        <f>COUNTIF(CreacionCuentaPersonas!A3:A23,"CreacionCuentaPersonas")</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="36">
-        <f>MAX(CreacionCuentaPersonas!C2:C61)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="36">
-        <f>MIN(CreacionCuentaPersonas!C2:C31)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="37">
-        <f>COUNTIF(CreacionCuentaPersonas!D3:D20,"SUCCES")</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="37">
-        <f>COUNTIF(CreacionCuentaPersonas!D3:D17,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="34">
-        <f>COUNTIF(CreacionCasoFelicitaciones!A4:A24,"creacionCasoFelicitaciones")</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="36">
-        <f>MAX(CreacionCasoFelicitaciones!C3:C62)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="36">
-        <f>MIN(CreacionCasoFelicitaciones!C3:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D4:D21,"SUCCES")</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D4:D18,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="34">
-        <f>COUNTIF(CreacionCasoInformacion!A5:A25,"creacionCasoInformacion")</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="36">
-        <f>MAX(CreacionCasoInformacion!C4:C63)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="36">
-        <f>MIN(CreacionCasoInformacion!C4:C33)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="37">
-        <f>COUNTIF(CreacionCasoInformacion!D5:D22,"SUCCES")</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="37">
-        <f>COUNTIF(CreacionCasoInformacion!D5:D19,"FAILED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="34">
-        <f>COUNTIF(creacionCasoQueja!A6:A26,"creacionCasoQueja")</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="36">
-        <f>MAX(creacionCasoQueja!C5:C64)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="36">
-        <f>MIN(creacionCasoQueja!C5:C34)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="37">
-        <f>COUNTIF(creacionCasoQueja!D6:D23,"SUCCES")</f>
-        <v>0</v>
-      </c>
       <c r="G10" s="37">
-        <f>COUNTIF(creacionCasoQueja!D6:D20,"FAILED")</f>
-        <v>0</v>
+        <f>COUNTIF(cuentaExistente!D2:D14,"FAILED")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>48</v>
+      <c r="B11" s="37" t="s">
+        <v>57</v>
       </c>
       <c r="C11" s="34">
-        <f>COUNTIF(creacionCasoSolicitud!A7:A27,"creacionCasoSolicitud")</f>
-        <v>0</v>
+        <f>COUNTIF(creaCuentaDesdeCasos!A2:A16,"creaCuentaDesdeCasos")</f>
+        <v>1</v>
       </c>
       <c r="D11" s="36">
-        <f>MAX(creacionCasoSolicitud!C6:C65)</f>
-        <v>0</v>
+        <f>MAX(creaCuentaDesdeCasos!C2:C22)</f>
+        <v>44895.000791342594</v>
       </c>
       <c r="E11" s="36">
-        <f>MIN(CreacionCasoFelicitaciones!C6:C35)</f>
-        <v>0</v>
+        <f>MIN(creaCuentaDesdeCasos!C2:C25)</f>
+        <v>44895.000791342594</v>
       </c>
       <c r="F11" s="37">
-        <f>COUNTIF(creacionCasoSolicitud!D7:D24,"SUCCES")</f>
-        <v>0</v>
+        <f>COUNTIF(creaCuentaDesdeCasos!D2:D21,"PASSED")</f>
+        <v>1</v>
       </c>
       <c r="G11" s="37">
-        <f>COUNTIF(creacionCasoSolicitud!D7:D21,"FAILED")</f>
+        <f>COUNTIF(creaCuentaDesdeCasos!D2:D15,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C12" s="34">
-        <f>COUNTIF(creacionCasoSugerencia!A8:A28,"creacionCasoSugerencia")</f>
+        <f>COUNTIF(CreacionCasoFelicitaciones!A2:A17,"CreacionCasoFelicitaciones")</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="36">
+        <f>MAX(CreacionCasoFelicitaciones!C2:C12)</f>
+        <v>44895.000289386575</v>
+      </c>
+      <c r="E12" s="36">
+        <f>MIN(CreacionCasoFelicitaciones!C2:C26)</f>
+        <v>44895.000289386575</v>
+      </c>
+      <c r="F12" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D22,"PASSED")</f>
         <v>0</v>
       </c>
-      <c r="D12" s="36">
-        <f>MAX(creacionCasoSugerencia!C7:C66)</f>
+      <c r="G12" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D16,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="34">
+        <f>COUNTIF(CreacionCasoInformacion!A2:A18,"CreacionCasoInformacion")</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="36">
+        <f>MAX(CreacionCasoInformacion!C2:C13)</f>
+        <v>44895.000761944444</v>
+      </c>
+      <c r="E13" s="36">
+        <f>MIN(CreacionCasoInformacion!C2:C27)</f>
+        <v>44895.000761944444</v>
+      </c>
+      <c r="F13" s="37">
+        <f>COUNTIF(CreacionCasoInformacion!D2:D23,"PASSED")</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="37">
+        <f>COUNTIF(CreacionCasoInformacion!D2:D17,"FAILED")</f>
         <v>0</v>
       </c>
-      <c r="E12" s="36">
-        <f>MIN(creacionCasoSugerencia!C7:C36)</f>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="34">
+        <f>COUNTIF(creacionCasoQueja!A2:A19,"CreacionCasoQueja")</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="36">
+        <f>MAX(creacionCasoQueja!C2:C14)</f>
+        <v>44895.000770451392</v>
+      </c>
+      <c r="E14" s="36">
+        <f>MIN(creacionCasoQueja!C2:C28)</f>
+        <v>44895.000770451392</v>
+      </c>
+      <c r="F14" s="37">
+        <f>COUNTIF(creacionCasoQueja!D2:D24,"PASSED")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="37">
-        <f>COUNTIF(creacionCasoSugerencia!D8:D25,"SUCCES")</f>
+      <c r="G14" s="37">
+        <f>COUNTIF(creacionCasoQueja!D2:D18,"FAILED")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="34">
+        <f>COUNTIF(creacionCasoSolicitud!A2:A20,"CreacionCasoSolicitud")</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="36">
+        <f>MAX(creacionCasoSolicitud!C2:C15)</f>
+        <v>44895.00081622685</v>
+      </c>
+      <c r="E15" s="36">
+        <f>MIN(creacionCasoSolicitud!C2:C29)</f>
+        <v>44895.00081622685</v>
+      </c>
+      <c r="F15" s="37">
+        <f>COUNTIF(creacionCasoSolicitud!D2:D25,"PASSED")</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="37">
+        <f>COUNTIF(creacionCasoSolicitud!D2:D19,"FAILED")</f>
         <v>0</v>
       </c>
-      <c r="G12" s="37">
-        <f>COUNTIF(creacionCasoSugerencia!D8:D22,"FAILED")</f>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="34">
+        <f>COUNTIF(creacionCasoSugerencia!A2:A21,"CreacionCasoSugerencia")</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="36">
+        <f>MAX(creacionCasoSugerencia!C2:C16)</f>
+        <v>44895.000819166664</v>
+      </c>
+      <c r="E16" s="36">
+        <f>MIN(creacionCasoSugerencia!C2:C30)</f>
+        <v>44895.000819166664</v>
+      </c>
+      <c r="F16" s="37">
+        <f>COUNTIF(creacionCasoSugerencia!D2:D26,"PASSED")</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="37">
+        <f>COUNTIF(creacionCasoSugerencia!D2:D20,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="24"/>
-      <c r="E15" s="31"/>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="24"/>
+      <c r="E19" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2047,11 +3049,303 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148A843F-DD9D-41C7-99B2-D4A8AA9201F5}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="86" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="51">
+        <v>44895.636384976853</v>
+      </c>
+      <c r="C2" s="52">
+        <v>44895.000122928242</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE742E0-6EA1-4AA0-8C3F-A539EF522416}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="87" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="53">
+        <v>44895.637012534724</v>
+      </c>
+      <c r="C2" s="54">
+        <v>44895.000157627313</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99C41C1-9AE8-4879-9151-AF8CDA72B09F}">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,15 +3370,25 @@
         <v>33</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="61">
+        <v>44895.644081956016</v>
+      </c>
+      <c r="C2" s="62">
+        <v>44895.000453946763</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
@@ -2310,12 +3614,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D82E4AC-5BDA-4423-B100-F014CDDF9FA5}">
   <dimension ref="A1:E401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,20 +3643,30 @@
         <v>33</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="59">
+        <v>44895.643136817132</v>
+      </c>
+      <c r="C2" s="60">
+        <v>44895.000818958331</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
     </row>
@@ -3998,12 +5312,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4BB373-E012-4B33-A2CA-3C06D5457D5C}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,20 +5341,30 @@
         <v>33</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="57">
+        <v>44895.639439652776</v>
+      </c>
+      <c r="C2" s="58">
+        <v>44895.000503796298</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
     </row>
@@ -4323,433 +5647,6 @@
       <c r="C43" s="30"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD12C50-8006-4482-89FC-B707702EBA26}">
-  <dimension ref="A1:E30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="91.85546875" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B796CB-0EB1-42DF-9E74-36B105845987}">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="80.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4759,20 +5656,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0E75C9-AD9E-493F-9E18-B1F69B9E3651}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFA25A7-D1EA-40A3-A54D-361605847836}">
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="85.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4789,20 +5685,30 @@
         <v>33</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="55">
+        <v>44895.638444259261</v>
+      </c>
+      <c r="C2" s="56">
+        <v>44895.000481504627</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
     </row>
@@ -4905,60 +5811,88 @@
       <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
cambios 1/12 -10 am
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alkosto\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91AB22-655C-41E2-84AE-06DBE16AA577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6466F6C-C38D-4A08-B885-A5147556D818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="2" activeTab="2" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="10" activeTab="14" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
@@ -32,9 +32,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CreacionCuentaEmpresa!$A$1:$E$16</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="95">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -281,6 +281,63 @@
   </si>
   <si>
     <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.38.30</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.22.22</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.28.45</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.31.36</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.34.50</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.46.10</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.48.26</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.51.43</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.53.16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.55.33</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.57.43</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.00.34</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.02.34</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.04.16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.06.29</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.08.32</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.11.31</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.13.37</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.16.59</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.19.41</t>
   </si>
 </sst>
 </file>
@@ -546,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -646,6 +703,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,11 +1063,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1075,8 +1170,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="84.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="84.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,18 +1209,38 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="103" t="n">
+        <v>44896.37719701389</v>
+      </c>
+      <c r="C3" s="104" t="n">
+        <v>44896.000382349535</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="105" t="n">
+        <v>44896.37889503472</v>
+      </c>
+      <c r="C4" s="106" t="n">
+        <v>44896.00090655093</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -1213,10 +1328,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="91.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="91.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,32 +1369,72 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="91" t="n">
+        <v>44896.36793449074</v>
+      </c>
+      <c r="C3" s="92" t="n">
+        <v>44896.00092760417</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="107" t="n">
+        <v>44896.38039679398</v>
+      </c>
+      <c r="C4" s="108" t="n">
+        <v>44896.000847256946</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="A5" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="113" t="n">
+        <v>44896.38484219908</v>
+      </c>
+      <c r="C5" s="114" t="n">
+        <v>44896.00034420139</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="A6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="115" t="n">
+        <v>44896.38769915509</v>
+      </c>
+      <c r="C6" s="116" t="n">
+        <v>44896.00087960648</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -1427,9 +1582,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="88.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="88.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,18 +1622,38 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="93" t="n">
+        <v>44896.369866168985</v>
+      </c>
+      <c r="C3" s="94" t="n">
+        <v>44896.000597893515</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="95" t="n">
+        <v>44896.37130587963</v>
+      </c>
+      <c r="C4" s="96" t="n">
+        <v>44896.0009587963</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -1660,11 +1835,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="82.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="82.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,39 +1877,89 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="87" t="n">
+        <v>44896.35836715278</v>
+      </c>
+      <c r="C3" s="88" t="n">
+        <v>44896.00082069445</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="89" t="n">
+        <v>44896.366354212965</v>
+      </c>
+      <c r="C4" s="90" t="n">
+        <v>44896.00093332176</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="A5" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="109" t="n">
+        <v>44896.38134674769</v>
+      </c>
+      <c r="C5" s="110" t="n">
+        <v>44896.00037087963</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="A6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="111" t="n">
+        <v>44896.38396199074</v>
+      </c>
+      <c r="C6" s="112" t="n">
+        <v>44896.00092774306</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="A7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="117" t="n">
+        <v>44896.38962021991</v>
+      </c>
+      <c r="C7" s="118" t="n">
+        <v>44896.000922928244</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -1879,8 +2104,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="82.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="82.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1918,18 +2143,38 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="97" t="n">
+        <v>44896.37239334491</v>
+      </c>
+      <c r="C3" s="98" t="n">
+        <v>44896.00046164352</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="99" t="n">
+        <v>44896.3744153588</v>
+      </c>
+      <c r="C4" s="100" t="n">
+        <v>44896.00097707176</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -2109,14 +2354,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63BF217-BF6E-441B-AE01-3F0540C3AB75}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="80.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="80.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2154,11 +2399,21 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="101" t="n">
+        <v>44896.376240578706</v>
+      </c>
+      <c r="C3" s="102" t="n">
+        <v>44896.00082158565</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
@@ -2431,10 +2686,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
@@ -2693,17 +2948,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E748D9-ED46-4D76-AD5F-92A006D16DD6}">
   <dimension ref="B3:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -3053,14 +3308,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="86" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="86.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,14 +3454,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="87" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="87.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3350,10 +3605,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="97.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="97.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3624,9 +3879,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="95.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="95.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5322,9 +5577,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="97.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="97.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5665,10 +5920,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="85.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="85.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5706,25 +5961,55 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="81" t="n">
+        <v>44896.34942479167</v>
+      </c>
+      <c r="C3" s="82" t="n">
+        <v>44896.00052267361</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="83" t="n">
+        <v>44896.35393858796</v>
+      </c>
+      <c r="C4" s="84" t="n">
+        <v>44896.00060251157</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="A5" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="85" t="n">
+        <v>44896.355975590275</v>
+      </c>
+      <c r="C5" s="86" t="n">
+        <v>44896.00065216435</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>

</xml_diff>

<commit_message>
cambios 1/12 - 10:30 am
</commit_message>
<xml_diff>
--- a/Indicadores.xlsx
+++ b/Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alkosto\everis-app-web-selenium-java-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6466F6C-C38D-4A08-B885-A5147556D818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927945E0-D5F5-47CF-996F-7AB9B2A06891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" firstSheet="10" activeTab="14" xr2:uid="{CC8ABF11-AA2D-4D04-8197-1986786B13BF}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
   <si>
     <t>Se busca una cuenta y si no existe se crea una tipo Empresa</t>
   </si>
@@ -235,109 +235,112 @@
     <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.16.11</t>
   </si>
   <si>
+    <t>CreacionCuentaPersonas</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.28.04</t>
+  </si>
+  <si>
+    <t>creacionCasoSugerencia</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.29.50</t>
+  </si>
+  <si>
+    <t>creacionCasoSolicitud</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.31.39</t>
+  </si>
+  <si>
+    <t>creacionCasoQueja</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.35.37</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.31.36</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.46.10</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.48.26</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.53.16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.57.43</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.00.34</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.04.16</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.06.29</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.11.31</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.16.59</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.19.41</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.52.04</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.57.19</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.59.15</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.00.19</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.01.51</t>
+  </si>
+  <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.17.03</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.18.38</t>
-  </si>
-  <si>
-    <t>CreacionCuentaPersonas</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.20.03</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.24.54</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.26.47</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.28.04</t>
-  </si>
-  <si>
-    <t>creacionCasoSugerencia</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.29.50</t>
-  </si>
-  <si>
-    <t>creacionCasoSolicitud</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.31.39</t>
-  </si>
-  <si>
-    <t>creacionCasoQueja</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.33.50</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.35.37</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\30.11.22_15.38.30</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.22.22</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.28.45</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.31.36</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.34.50</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.46.10</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.48.26</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.51.43</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.53.16</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.55.33</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_08.57.43</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.00.34</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.02.34</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.04.16</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.06.29</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.08.32</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.11.31</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.13.37</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.16.59</t>
-  </si>
-  <si>
-    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_09.19.41</t>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.03.43</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.05.24</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.07.14</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.08.49</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.10.34</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.12.45</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.14.32</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.17.39</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.20.53</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.23.01</t>
+  </si>
+  <si>
+    <t>C:\Alkosto\everis-app-web-selenium-java-master\reportes\indicadores\01.12.22_10.24.54</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -652,9 +655,29 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -703,14 +726,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1071,13 +1086,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="97"/>
     </row>
     <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F4" s="13" t="s">
@@ -1162,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB547C11-8059-4516-AEFD-2AA57D4205D1}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,51 +1210,51 @@
       <c r="A2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="59">
         <v>44895.645306481485</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="60">
         <v>44895.000791342594</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="103" t="n">
-        <v>44896.37719701389</v>
-      </c>
-      <c r="C3" s="104" t="n">
-        <v>44896.000382349535</v>
+      <c r="B3" s="83">
+        <v>44896.378895034723</v>
+      </c>
+      <c r="C3" s="84">
+        <v>44896.000906550929</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="105" t="n">
-        <v>44896.37889503472</v>
-      </c>
-      <c r="C4" s="106" t="n">
-        <v>44896.00090655093</v>
+      <c r="B4" s="117" t="n">
+        <v>44896.42498065972</v>
+      </c>
+      <c r="C4" s="118" t="n">
+        <v>44896.00093760416</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1304,13 +1319,6 @@
       <c r="C13" s="30"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1320,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD12C50-8006-4482-89FC-B707702EBA26}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,86 +1363,76 @@
       <c r="A2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="73">
-        <v>44895.652058402775</v>
-      </c>
-      <c r="C2" s="74">
-        <v>44895.000289386575</v>
+      <c r="B2" s="75">
+        <v>44896.367934490743</v>
+      </c>
+      <c r="C2" s="76">
+        <v>44896.000927604167</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="91" t="n">
-        <v>44896.36793449074</v>
-      </c>
-      <c r="C3" s="92" t="n">
-        <v>44896.00092760417</v>
+      <c r="B3" s="85">
+        <v>44896.380396793982</v>
+      </c>
+      <c r="C3" s="86">
+        <v>44896.000847256946</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="107" t="n">
-        <v>44896.38039679398</v>
-      </c>
-      <c r="C4" s="108" t="n">
-        <v>44896.000847256946</v>
+      <c r="B4" s="89">
+        <v>44896.387699155093</v>
+      </c>
+      <c r="C4" s="90">
+        <v>44896.000879606479</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="113" t="n">
-        <v>44896.38484219908</v>
-      </c>
-      <c r="C5" s="114" t="n">
-        <v>44896.00034420139</v>
+      <c r="B5" s="129" t="n">
+        <v>44896.4347787963</v>
+      </c>
+      <c r="C5" s="130" t="n">
+        <v>44896.00080618056</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="115" t="n">
-        <v>44896.38769915509</v>
-      </c>
-      <c r="C6" s="116" t="n">
-        <v>44896.00087960648</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>93</v>
-      </c>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -1500,70 +1498,56 @@
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="38"/>
       <c r="C18" s="39"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="38"/>
       <c r="C19" s="39"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="38"/>
       <c r="C20" s="39"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="38"/>
       <c r="C21" s="39"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="38"/>
       <c r="C22" s="39"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="38"/>
       <c r="C23" s="39"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="38"/>
       <c r="C24" s="39"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="38"/>
       <c r="C25" s="39"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="38"/>
       <c r="C26" s="39"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="38"/>
       <c r="C27" s="39"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="38"/>
       <c r="C28" s="39"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1574,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B796CB-0EB1-42DF-9E74-36B105845987}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,51 +1592,51 @@
       <c r="A2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="65">
         <v>44895.650510613428</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="66">
         <v>44895.000761944444</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="93" t="n">
-        <v>44896.369866168985</v>
-      </c>
-      <c r="C3" s="94" t="n">
-        <v>44896.000597893515</v>
+      <c r="B3" s="77">
+        <v>44896.371305879627</v>
+      </c>
+      <c r="C3" s="78">
+        <v>44896.0009587963</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="95" t="n">
-        <v>44896.37130587963</v>
-      </c>
-      <c r="C4" s="96" t="n">
-        <v>44896.0009587963</v>
+      <c r="B4" s="127" t="n">
+        <v>44896.43353643519</v>
+      </c>
+      <c r="C4" s="128" t="n">
+        <v>44896.000859988424</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,70 +1723,67 @@
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="40"/>
       <c r="C18" s="41"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="40"/>
       <c r="C20" s="41"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="40"/>
       <c r="C23" s="41"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="40"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="40"/>
       <c r="C27" s="41"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
       <c r="C28" s="41"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="40"/>
       <c r="C29" s="41"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="40"/>
       <c r="C30" s="41"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="40"/>
       <c r="C31" s="41"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="40"/>
       <c r="C32" s="41"/>
     </row>
@@ -1813,10 +1794,6 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="40"/>
       <c r="C34" s="41"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1827,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0E75C9-AD9E-493F-9E18-B1F69B9E3651}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,105 +1838,95 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="69">
-        <v>44895.649289513887</v>
-      </c>
-      <c r="C2" s="70">
-        <v>44895.000770451392</v>
+        <v>66</v>
+      </c>
+      <c r="B2" s="73">
+        <v>44896.366354212965</v>
+      </c>
+      <c r="C2" s="74">
+        <v>44896.00093332176</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="87" t="n">
-        <v>44896.35836715278</v>
-      </c>
-      <c r="C3" s="88" t="n">
-        <v>44896.00082069445</v>
+        <v>66</v>
+      </c>
+      <c r="B3" s="87">
+        <v>44896.383961990738</v>
+      </c>
+      <c r="C3" s="88">
+        <v>44896.000927743058</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="89" t="n">
-        <v>44896.366354212965</v>
-      </c>
-      <c r="C4" s="90" t="n">
-        <v>44896.00093332176</v>
+        <v>66</v>
+      </c>
+      <c r="B4" s="91">
+        <v>44896.38962021991</v>
+      </c>
+      <c r="C4" s="92">
+        <v>44896.000922928244</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="109" t="n">
-        <v>44896.38134674769</v>
-      </c>
-      <c r="C5" s="110" t="n">
-        <v>44896.00037087963</v>
+        <v>66</v>
+      </c>
+      <c r="B5" s="93">
+        <v>44896.412131435187</v>
+      </c>
+      <c r="C5" s="94">
+        <v>44896.000948923611</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="111" t="n">
-        <v>44896.38396199074</v>
-      </c>
-      <c r="C6" s="112" t="n">
-        <v>44896.00092774306</v>
+        <v>66</v>
+      </c>
+      <c r="B6" s="125" t="n">
+        <v>44896.432136655094</v>
+      </c>
+      <c r="C6" s="126" t="n">
+        <v>44896.00093681713</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="117" t="n">
-        <v>44896.38962021991</v>
-      </c>
-      <c r="C7" s="118" t="n">
-        <v>44896.000922928244</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>94</v>
-      </c>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -2011,81 +1978,60 @@
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="40"/>
       <c r="C18" s="41"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="40"/>
       <c r="C20" s="41"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="40"/>
       <c r="C23" s="41"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="40"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="40"/>
       <c r="C27" s="41"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
       <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2096,10 +2042,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DF4948-357F-40F6-A41C-D62917141212}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,61 +2073,71 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="67">
+        <v>64</v>
+      </c>
+      <c r="B2" s="63">
         <v>44895.64780835648</v>
       </c>
-      <c r="C2" s="68">
+      <c r="C2" s="64">
         <v>44895.00081622685</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="97" t="n">
-        <v>44896.37239334491</v>
-      </c>
-      <c r="C3" s="98" t="n">
-        <v>44896.00046164352</v>
+        <v>64</v>
+      </c>
+      <c r="B3" s="79">
+        <v>44896.374415358798</v>
+      </c>
+      <c r="C3" s="80">
+        <v>44896.000977071759</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="99" t="n">
-        <v>44896.3744153588</v>
-      </c>
-      <c r="C4" s="100" t="n">
-        <v>44896.00097707176</v>
+        <v>64</v>
+      </c>
+      <c r="B4" s="121" t="n">
+        <v>44896.427201493054</v>
+      </c>
+      <c r="C4" s="122" t="n">
+        <v>44896.00039451389</v>
       </c>
       <c r="D4" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="123" t="n">
+        <v>44896.42993957176</v>
+      </c>
+      <c r="C5" s="124" t="n">
+        <v>44896.00099202546</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="E5" s="28" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
@@ -2260,70 +2216,67 @@
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="40"/>
       <c r="C18" s="41"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="40"/>
       <c r="C20" s="41"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="40"/>
       <c r="C23" s="41"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="40"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="40"/>
       <c r="C27" s="41"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
       <c r="C28" s="41"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="40"/>
       <c r="C29" s="41"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="40"/>
       <c r="C30" s="41"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="40"/>
       <c r="C31" s="41"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="40"/>
       <c r="C32" s="41"/>
     </row>
@@ -2338,10 +2291,6 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="40"/>
       <c r="C35" s="41"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2383,44 +2332,54 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="65">
+        <v>62</v>
+      </c>
+      <c r="B2" s="61">
         <v>44895.646562002315</v>
       </c>
-      <c r="C2" s="66">
+      <c r="C2" s="62">
         <v>44895.000819166664</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="101" t="n">
+        <v>62</v>
+      </c>
+      <c r="B3" s="81">
         <v>44896.376240578706</v>
       </c>
-      <c r="C3" s="102" t="n">
-        <v>44896.00082158565</v>
+      <c r="C3" s="82">
+        <v>44896.000821585651</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="119" t="n">
+        <v>44896.42636859954</v>
+      </c>
+      <c r="C4" s="120" t="n">
+        <v>44896.00081993055</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -2717,7 +2676,7 @@
       </c>
     </row>
     <row r="3" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="98" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2735,7 +2694,7 @@
       </c>
     </row>
     <row r="4" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
+      <c r="A4" s="99"/>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +2710,7 @@
       </c>
     </row>
     <row r="5" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="99"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -2764,7 +2723,7 @@
       </c>
     </row>
     <row r="6" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
+      <c r="A6" s="99"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -2777,7 +2736,7 @@
       </c>
     </row>
     <row r="7" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
+      <c r="A7" s="99"/>
       <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
@@ -2789,7 +2748,7 @@
       </c>
     </row>
     <row r="8" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
+      <c r="A8" s="99"/>
       <c r="B8" s="6" t="s">
         <v>45</v>
       </c>
@@ -2802,7 +2761,7 @@
       </c>
     </row>
     <row r="9" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="99"/>
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
@@ -2815,7 +2774,7 @@
       </c>
     </row>
     <row r="10" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
+      <c r="A10" s="99"/>
       <c r="B10" s="6" t="s">
         <v>51</v>
       </c>
@@ -2828,8 +2787,8 @@
       </c>
     </row>
     <row r="11" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="99"/>
+      <c r="B11" s="42" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -2841,7 +2800,7 @@
       </c>
     </row>
     <row r="12" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="80"/>
+      <c r="A12" s="100"/>
       <c r="B12" s="6" t="s">
         <v>52</v>
       </c>
@@ -2854,7 +2813,7 @@
       </c>
     </row>
     <row r="13" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -2870,7 +2829,7 @@
       </c>
     </row>
     <row r="14" spans="1:4 16383:16383" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
+      <c r="A14" s="99"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -2883,7 +2842,7 @@
       </c>
     </row>
     <row r="15" spans="1:4 16383:16383" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="7" t="s">
         <v>3</v>
       </c>
@@ -2949,7 +2908,7 @@
   <dimension ref="B3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+      <selection activeCell="G5" sqref="G5:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,13 +2921,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="77"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="97"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
@@ -3021,15 +2980,15 @@
       </c>
       <c r="C6" s="34">
         <f>COUNTIF(inicioSesionFallido!A2:A17,"inicioSesionFallido")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="35">
         <f>MAX(inicioSesionFallido!C2:C95)</f>
-        <v>44895.000157627313</v>
+        <v>0</v>
       </c>
       <c r="E6" s="36">
         <f>MIN(inicioSesionFallido!C2:C21)</f>
-        <v>44895.000157627313</v>
+        <v>0</v>
       </c>
       <c r="F6" s="37">
         <f>COUNTIF(inicioSesionFallido!D2:D18,"PASSED")</f>
@@ -3037,7 +2996,7 @@
       </c>
       <c r="G6" s="37">
         <f>COUNTIF(inicioSesionFallido!D2:D22,"FAILED")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3046,15 +3005,15 @@
       </c>
       <c r="C7" s="34">
         <f>COUNTIF(CreacionCuentaAliados!A2:A17,"CreacionCuentaAliados")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="35">
         <f>MAX(CreacionCuentaAliados!C2:C95)</f>
-        <v>44895.000453946763</v>
+        <v>0</v>
       </c>
       <c r="E7" s="36">
         <f>MIN(CreacionCuentaAliados!C2:C21)</f>
-        <v>44895.000453946763</v>
+        <v>0</v>
       </c>
       <c r="F7" s="37">
         <f>COUNTIF(CreacionCuentaAliados!D2:D18,"SUCCES")</f>
@@ -3062,7 +3021,7 @@
       </c>
       <c r="G7" s="37">
         <f>COUNTIF(CreacionCuentaAliados!D2:D22,"FAILED")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3071,15 +3030,15 @@
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(CreacionCuentaEmpresa!A2:A13,"CreacionCuentaEmpresa")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="36">
         <f>MAX(CreacionCuentaEmpresa!C2:C8)</f>
-        <v>44895.000818958331</v>
+        <v>0</v>
       </c>
       <c r="E8" s="36">
         <f>MIN(CreacionCuentaEmpresa!C2:C22)</f>
-        <v>44895.000818958331</v>
+        <v>0</v>
       </c>
       <c r="F8" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D18,"PASSED")</f>
@@ -3087,24 +3046,24 @@
       </c>
       <c r="G8" s="37">
         <f>COUNTIF(CreacionCuentaEmpresa!D2:D12,"FAILED")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(CreacionCuentaPersonas!A2:A14,"CreacionCuentaPersonas")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="36">
         <f>MAX(CreacionCuentaPersonas!C2:C8)</f>
-        <v>44895.000503796298</v>
+        <v>0</v>
       </c>
       <c r="E9" s="36">
         <f>MIN(CreacionCuentaPersonas!C2:C23)</f>
-        <v>44895.000503796298</v>
+        <v>0</v>
       </c>
       <c r="F9" s="37">
         <f>COUNTIF(CreacionCuentaPersonas!D2:D19,"PASSED")</f>
@@ -3112,7 +3071,7 @@
       </c>
       <c r="G9" s="37">
         <f>COUNTIF(CreacionCuentaPersonas!D2:D13,"FAILED")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3125,19 +3084,19 @@
       </c>
       <c r="D10" s="36">
         <f>MAX(cuentaExistente!C2:C10)</f>
-        <v>44895.000481504627</v>
+        <v>44896.000652164352</v>
       </c>
       <c r="E10" s="36">
         <f>MIN(cuentaExistente!C2:C24)</f>
-        <v>44895.000481504627</v>
+        <v>44896.000652164352</v>
       </c>
       <c r="F10" s="37">
         <f>COUNTIF(cuentaExistente!D2:D20,"PASSED")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="37">
         <f>COUNTIF(cuentaExistente!D2:D14,"FAILED")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3145,23 +3104,23 @@
         <v>57</v>
       </c>
       <c r="C11" s="34">
-        <f>COUNTIF(creaCuentaDesdeCasos!A2:A16,"creaCuentaDesdeCasos")</f>
-        <v>1</v>
+        <f>COUNTIF(creaCuentaDesdeCasos!A2:A15,"creaCuentaDesdeCasos")</f>
+        <v>2</v>
       </c>
       <c r="D11" s="36">
-        <f>MAX(creaCuentaDesdeCasos!C2:C22)</f>
+        <f>MAX(creaCuentaDesdeCasos!C2:C21)</f>
+        <v>44896.000906550929</v>
+      </c>
+      <c r="E11" s="36">
+        <f>MIN(creaCuentaDesdeCasos!C2:C24)</f>
         <v>44895.000791342594</v>
       </c>
-      <c r="E11" s="36">
-        <f>MIN(creaCuentaDesdeCasos!C2:C25)</f>
-        <v>44895.000791342594</v>
-      </c>
       <c r="F11" s="37">
-        <f>COUNTIF(creaCuentaDesdeCasos!D2:D21,"PASSED")</f>
-        <v>1</v>
+        <f>COUNTIF(creaCuentaDesdeCasos!D2:D20,"PASSED")</f>
+        <v>2</v>
       </c>
       <c r="G11" s="37">
-        <f>COUNTIF(creaCuentaDesdeCasos!D2:D15,"FAILED")</f>
+        <f>COUNTIF(creaCuentaDesdeCasos!D2:D14,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
@@ -3170,24 +3129,24 @@
         <v>43</v>
       </c>
       <c r="C12" s="34">
-        <f>COUNTIF(CreacionCasoFelicitaciones!A2:A17,"CreacionCasoFelicitaciones")</f>
-        <v>1</v>
+        <f>COUNTIF(CreacionCasoFelicitaciones!A2:A15,"CreacionCasoFelicitaciones")</f>
+        <v>3</v>
       </c>
       <c r="D12" s="36">
-        <f>MAX(CreacionCasoFelicitaciones!C2:C12)</f>
-        <v>44895.000289386575</v>
+        <f>MAX(CreacionCasoFelicitaciones!C2:C10)</f>
+        <v>44896.000927604167</v>
       </c>
       <c r="E12" s="36">
-        <f>MIN(CreacionCasoFelicitaciones!C2:C26)</f>
-        <v>44895.000289386575</v>
+        <f>MIN(CreacionCasoFelicitaciones!C2:C24)</f>
+        <v>44896.000847256946</v>
       </c>
       <c r="F12" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D22,"PASSED")</f>
+        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D20,"PASSED")</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="37">
+        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D14,"FAILED")</f>
         <v>0</v>
-      </c>
-      <c r="G12" s="37">
-        <f>COUNTIF(CreacionCasoFelicitaciones!D2:D16,"FAILED")</f>
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3195,23 +3154,23 @@
         <v>44</v>
       </c>
       <c r="C13" s="34">
-        <f>COUNTIF(CreacionCasoInformacion!A2:A18,"CreacionCasoInformacion")</f>
-        <v>1</v>
+        <f>COUNTIF(CreacionCasoInformacion!A2:A17,"CreacionCasoInformacion")</f>
+        <v>2</v>
       </c>
       <c r="D13" s="36">
-        <f>MAX(CreacionCasoInformacion!C2:C13)</f>
+        <f>MAX(CreacionCasoInformacion!C2:C12)</f>
+        <v>44896.0009587963</v>
+      </c>
+      <c r="E13" s="36">
+        <f>MIN(CreacionCasoInformacion!C2:C26)</f>
         <v>44895.000761944444</v>
       </c>
-      <c r="E13" s="36">
-        <f>MIN(CreacionCasoInformacion!C2:C27)</f>
-        <v>44895.000761944444</v>
-      </c>
       <c r="F13" s="37">
-        <f>COUNTIF(CreacionCasoInformacion!D2:D23,"PASSED")</f>
-        <v>1</v>
+        <f>COUNTIF(CreacionCasoInformacion!D2:D22,"PASSED")</f>
+        <v>2</v>
       </c>
       <c r="G13" s="37">
-        <f>COUNTIF(CreacionCasoInformacion!D2:D17,"FAILED")</f>
+        <f>COUNTIF(CreacionCasoInformacion!D2:D16,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
@@ -3220,24 +3179,24 @@
         <v>46</v>
       </c>
       <c r="C14" s="34">
-        <f>COUNTIF(creacionCasoQueja!A2:A19,"CreacionCasoQueja")</f>
-        <v>1</v>
+        <f>COUNTIF(creacionCasoQueja!A2:A16,"CreacionCasoQueja")</f>
+        <v>4</v>
       </c>
       <c r="D14" s="36">
-        <f>MAX(creacionCasoQueja!C2:C14)</f>
-        <v>44895.000770451392</v>
+        <f>MAX(creacionCasoQueja!C2:C11)</f>
+        <v>44896.000948923611</v>
       </c>
       <c r="E14" s="36">
-        <f>MIN(creacionCasoQueja!C2:C28)</f>
-        <v>44895.000770451392</v>
+        <f>MIN(creacionCasoQueja!C2:C25)</f>
+        <v>44896.000922928244</v>
       </c>
       <c r="F14" s="37">
-        <f>COUNTIF(creacionCasoQueja!D2:D24,"PASSED")</f>
+        <f>COUNTIF(creacionCasoQueja!D2:D21,"PASSED")</f>
+        <v>4</v>
+      </c>
+      <c r="G14" s="37">
+        <f>COUNTIF(creacionCasoQueja!D2:D15,"FAILED")</f>
         <v>0</v>
-      </c>
-      <c r="G14" s="37">
-        <f>COUNTIF(creacionCasoQueja!D2:D18,"FAILED")</f>
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3245,23 +3204,23 @@
         <v>47</v>
       </c>
       <c r="C15" s="34">
-        <f>COUNTIF(creacionCasoSolicitud!A2:A20,"CreacionCasoSolicitud")</f>
-        <v>1</v>
+        <f>COUNTIF(creacionCasoSolicitud!A2:A19,"CreacionCasoSolicitud")</f>
+        <v>2</v>
       </c>
       <c r="D15" s="36">
-        <f>MAX(creacionCasoSolicitud!C2:C15)</f>
+        <f>MAX(creacionCasoSolicitud!C2:C14)</f>
+        <v>44896.000977071759</v>
+      </c>
+      <c r="E15" s="36">
+        <f>MIN(creacionCasoSolicitud!C2:C28)</f>
         <v>44895.00081622685</v>
       </c>
-      <c r="E15" s="36">
-        <f>MIN(creacionCasoSolicitud!C2:C29)</f>
-        <v>44895.00081622685</v>
-      </c>
       <c r="F15" s="37">
-        <f>COUNTIF(creacionCasoSolicitud!D2:D25,"PASSED")</f>
-        <v>1</v>
+        <f>COUNTIF(creacionCasoSolicitud!D2:D24,"PASSED")</f>
+        <v>2</v>
       </c>
       <c r="G15" s="37">
-        <f>COUNTIF(creacionCasoSolicitud!D2:D19,"FAILED")</f>
+        <f>COUNTIF(creacionCasoSolicitud!D2:D18,"FAILED")</f>
         <v>0</v>
       </c>
     </row>
@@ -3271,11 +3230,11 @@
       </c>
       <c r="C16" s="34">
         <f>COUNTIF(creacionCasoSugerencia!A2:A21,"CreacionCasoSugerencia")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="36">
         <f>MAX(creacionCasoSugerencia!C2:C16)</f>
-        <v>44895.000819166664</v>
+        <v>44896.000821585651</v>
       </c>
       <c r="E16" s="36">
         <f>MIN(creacionCasoSugerencia!C2:C30)</f>
@@ -3283,7 +3242,7 @@
       </c>
       <c r="F16" s="37">
         <f>COUNTIF(creacionCasoSugerencia!D2:D26,"PASSED")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="37">
         <f>COUNTIF(creacionCasoSugerencia!D2:D20,"FAILED")</f>
@@ -3308,7 +3267,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3339,10 +3298,10 @@
       <c r="A2" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="47">
         <v>44895.636384976853</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="48">
         <v>44895.000122928242</v>
       </c>
       <c r="D2" s="28" t="s">
@@ -3353,11 +3312,21 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="101" t="n">
+        <v>44896.414982835646</v>
+      </c>
+      <c r="C3" s="102" t="n">
+        <v>44896.000149837964</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
@@ -3454,7 +3423,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,17 +3454,17 @@
       <c r="A2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="53">
-        <v>44895.637012534724</v>
-      </c>
-      <c r="C2" s="54">
-        <v>44895.000157627313</v>
+      <c r="B2" s="103" t="n">
+        <v>44896.416324247686</v>
+      </c>
+      <c r="C2" s="104" t="n">
+        <v>44896.00016091435</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3600,7 +3569,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E15"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,17 +3601,17 @@
       <c r="A2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="61">
-        <v>44895.644081956016</v>
-      </c>
-      <c r="C2" s="62">
-        <v>44895.000453946763</v>
+      <c r="B2" s="115" t="n">
+        <v>44896.42348508102</v>
+      </c>
+      <c r="C2" s="116" t="n">
+        <v>44896.00066952546</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,7 +3843,7 @@
   <dimension ref="A1:E401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,32 +3874,52 @@
       <c r="A2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="59">
-        <v>44895.643136817132</v>
-      </c>
-      <c r="C2" s="60">
-        <v>44895.000818958331</v>
+      <c r="B2" s="109" t="n">
+        <v>44896.420148460646</v>
+      </c>
+      <c r="C2" s="110" t="n">
+        <v>44896.0008716088</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="111" t="n">
+        <v>44896.42117847222</v>
+      </c>
+      <c r="C3" s="112" t="n">
+        <v>44896.00072150463</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="113" t="n">
+        <v>44896.422405150464</v>
+      </c>
+      <c r="C4" s="114" t="n">
+        <v>44896.00068042824</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
@@ -5572,7 +5561,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5601,25 +5590,25 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="57">
-        <v>44895.639439652776</v>
-      </c>
-      <c r="C2" s="58">
-        <v>44895.000503796298</v>
+        <v>60</v>
+      </c>
+      <c r="B2" s="107" t="n">
+        <v>44896.41871104167</v>
+      </c>
+      <c r="C2" s="108" t="n">
+        <v>44896.00072053241</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
     </row>
@@ -5915,7 +5904,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5947,68 +5936,48 @@
       <c r="A2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="55">
-        <v>44895.638444259261</v>
-      </c>
-      <c r="C2" s="56">
-        <v>44895.000481504627</v>
+      <c r="B2" s="105" t="n">
+        <v>44896.41741083333</v>
+      </c>
+      <c r="C2" s="106" t="n">
+        <v>44896.00050657408</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="81" t="n">
-        <v>44896.34942479167</v>
-      </c>
-      <c r="C3" s="82" t="n">
-        <v>44896.00052267361</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>76</v>
-      </c>
+      <c r="A3" s="28"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="83" t="n">
-        <v>44896.35393858796</v>
-      </c>
-      <c r="C4" s="84" t="n">
-        <v>44896.00060251157</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>77</v>
-      </c>
+      <c r="A4" s="28"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="85" t="n">
+      <c r="B5" s="71">
         <v>44896.355975590275</v>
       </c>
-      <c r="C5" s="86" t="n">
-        <v>44896.00065216435</v>
+      <c r="C5" s="72">
+        <v>44896.000652164352</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6097,85 +6066,85 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="48"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
     </row>

</xml_diff>